<commit_message>
The big necessary update ReadMe (+BOAT/WOAT)
Updated the ReadMe + added BOAT/WOAT section to it
</commit_message>
<xml_diff>
--- a/rsc/teams/BOAT and WOAT.xlsx
+++ b/rsc/teams/BOAT and WOAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Documents\GitHub\CFBPoll\rsc\teams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED684F2B-44BE-4AC8-9817-7ABAE11F0BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DA05E3-7023-410F-8EE2-F9C3EB20F2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD7DC722-BCA6-480D-9BEB-13AA7385FFC0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Auburn</t>
   </si>
@@ -111,6 +111,42 @@
   </si>
   <si>
     <t>Army</t>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>12-0</t>
+  </si>
+  <si>
+    <t>13-0</t>
+  </si>
+  <si>
+    <t>13-1</t>
+  </si>
+  <si>
+    <t>12-1</t>
+  </si>
+  <si>
+    <t>14-0</t>
+  </si>
+  <si>
+    <t>15-0</t>
+  </si>
+  <si>
+    <t>14-1</t>
+  </si>
+  <si>
+    <t>0-12</t>
+  </si>
+  <si>
+    <t>0-11</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>1-11</t>
   </si>
 </sst>
 </file>
@@ -158,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -166,6 +202,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,31 +523,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8117188-CCB6-4F70-99F0-65941D6F0E4C}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -515,17 +559,23 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -535,17 +585,23 @@
       <c r="C3">
         <v>42.308999999999997</v>
       </c>
-      <c r="F3">
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3">
         <v>2001</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>15.052</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2002</v>
       </c>
@@ -555,17 +611,23 @@
       <c r="C4">
         <v>40.369</v>
       </c>
-      <c r="F4">
+      <c r="D4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4">
         <v>2002</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>15.397</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2004</v>
       </c>
@@ -575,17 +637,23 @@
       <c r="C5" s="1">
         <v>40.537999999999997</v>
       </c>
-      <c r="F5">
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
         <v>2002</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>14.945</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2004</v>
       </c>
@@ -595,17 +663,23 @@
       <c r="C6" s="1">
         <v>40.426000000000002</v>
       </c>
-      <c r="F6">
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6">
         <v>2004</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>13.954000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2006</v>
       </c>
@@ -615,17 +689,23 @@
       <c r="C7" s="1">
         <v>40.57</v>
       </c>
-      <c r="F7">
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
         <v>2006</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>15.904</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -635,17 +715,23 @@
       <c r="C8" s="1">
         <v>40.69</v>
       </c>
-      <c r="F8">
+      <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8">
         <v>2006</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>14.394</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -655,17 +741,23 @@
       <c r="C9" s="1">
         <v>41.131</v>
       </c>
-      <c r="F9">
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9">
         <v>2012</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>15.877000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2011</v>
       </c>
@@ -675,17 +767,23 @@
       <c r="C10" s="1">
         <v>40.085000000000001</v>
       </c>
-      <c r="F10">
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
         <v>2012</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>15.510999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -695,17 +793,23 @@
       <c r="C11" s="1">
         <v>40.396000000000001</v>
       </c>
-      <c r="F11">
+      <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11">
         <v>2013</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>13.973000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2018</v>
       </c>
@@ -715,17 +819,23 @@
       <c r="C12" s="4">
         <v>42.445</v>
       </c>
-      <c r="F12">
+      <c r="D12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
         <v>2018</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>15.353999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2018</v>
       </c>
@@ -735,17 +845,23 @@
       <c r="C13" s="1">
         <v>40.396999999999998</v>
       </c>
-      <c r="F13">
+      <c r="D13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13">
         <v>2019</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>15.371</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2019</v>
       </c>
@@ -755,17 +871,23 @@
       <c r="C14" s="1">
         <v>42.374000000000002</v>
       </c>
-      <c r="F14">
+      <c r="D14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14">
         <v>2019</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>14.526999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -775,22 +897,31 @@
       <c r="C15" s="1">
         <v>40.267000000000003</v>
       </c>
-      <c r="F15" s="3">
+      <c r="D15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="3">
         <v>2019</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="4">
         <v>13.37</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Poll of the 2020 Season
It's out!  New additions to BOAT and WOAT!
</commit_message>
<xml_diff>
--- a/rsc/teams/BOAT and WOAT.xlsx
+++ b/rsc/teams/BOAT and WOAT.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Documents\GitHub\CFBPoll\rsc\teams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1E0D31-5BE3-4AA0-9866-5E210A68B2CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70425F50-CFDF-4D20-A4B5-CA66E6976E28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD7DC722-BCA6-480D-9BEB-13AA7385FFC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD7DC722-BCA6-480D-9BEB-13AA7385FFC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$U$14:$X$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$S$2:$V$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="54">
   <si>
     <t>Auburn</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>Worst of all Time (Playoff Era)</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
+  <si>
+    <t>Vanderbilt</t>
+  </si>
+  <si>
+    <t>0-9</t>
   </si>
 </sst>
 </file>
@@ -576,7 +588,7 @@
   <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +597,10 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -605,8 +621,8 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="1">
-        <f>AVERAGE(I3:I11)</f>
-        <v>41.076555555555551</v>
+        <f>AVERAGE(I3:I12)</f>
+        <v>41.055499999999995</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>48</v>
@@ -625,8 +641,8 @@
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="1">
-        <f>AVERAGE(U3:U11)</f>
-        <v>15.015285714285714</v>
+        <f>AVERAGE(U3:U12)</f>
+        <v>15.1547</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -817,16 +833,16 @@
         <v>32</v>
       </c>
       <c r="S5">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="T5" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="U5" s="1">
-        <v>15.226000000000001</v>
+        <v>15.04</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -867,13 +883,13 @@
         <v>32</v>
       </c>
       <c r="S6">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="T6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="U6" s="1">
-        <v>15.353999999999999</v>
+        <v>15.226000000000001</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>35</v>
@@ -917,13 +933,13 @@
         <v>32</v>
       </c>
       <c r="S7">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="T7" t="s">
         <v>18</v>
       </c>
       <c r="U7" s="1">
-        <v>15.371</v>
+        <v>15.353999999999999</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>35</v>
@@ -943,16 +959,16 @@
         <v>27</v>
       </c>
       <c r="G8">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="1">
-        <v>40.396999999999998</v>
+        <v>40.866</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="M8">
         <v>2005</v>
@@ -967,16 +983,16 @@
         <v>32</v>
       </c>
       <c r="S8">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="T8" t="s">
         <v>18</v>
       </c>
       <c r="U8" s="1">
-        <v>15.507</v>
+        <v>15.371</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -993,16 +1009,16 @@
         <v>39</v>
       </c>
       <c r="G9">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
       </c>
       <c r="I9" s="1">
-        <v>40.344999999999999</v>
+        <v>40.396999999999998</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="M9">
         <v>2002</v>
@@ -1017,13 +1033,13 @@
         <v>35</v>
       </c>
       <c r="S9">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="T9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="U9" s="1">
-        <v>15.752000000000001</v>
+        <v>15.507</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>32</v>
@@ -1043,13 +1059,13 @@
         <v>27</v>
       </c>
       <c r="G10">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I10" s="1">
-        <v>40.267000000000003</v>
+        <v>40.344999999999999</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>27</v>
@@ -1065,6 +1081,18 @@
       </c>
       <c r="P10" s="5" t="s">
         <v>37</v>
+      </c>
+      <c r="S10">
+        <v>2020</v>
+      </c>
+      <c r="T10" t="s">
+        <v>51</v>
+      </c>
+      <c r="U10" s="1">
+        <v>15.61</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1081,16 +1109,16 @@
         <v>27</v>
       </c>
       <c r="G11">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="H11" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="1">
-        <v>40.140999999999998</v>
+        <v>40.267000000000003</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M11">
         <v>2005</v>
@@ -1103,6 +1131,18 @@
       </c>
       <c r="P11" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="S11">
+        <v>2015</v>
+      </c>
+      <c r="T11" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="1">
+        <v>15.752000000000001</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1118,8 +1158,18 @@
       <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="5"/>
+      <c r="G12">
+        <v>2014</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1">
+        <v>40.140999999999998</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="M12">
         <v>2001</v>
       </c>
@@ -1131,6 +1181,18 @@
       </c>
       <c r="P12" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="S12">
+        <v>2020</v>
+      </c>
+      <c r="T12" t="s">
+        <v>15</v>
+      </c>
+      <c r="U12" s="1">
+        <v>15.79</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1146,8 +1208,6 @@
       <c r="D13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="5"/>
       <c r="M13">
         <v>2003</v>
       </c>
@@ -1257,8 +1317,6 @@
       <c r="X16" s="5"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="5"/>
       <c r="M17">
         <v>2012</v>
       </c>

</xml_diff>